<commit_message>
Removing molten changed the number of rows.
</commit_message>
<xml_diff>
--- a/Macro/Reference.xlsx
+++ b/Macro/Reference.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cliff\OneDrive\Documents\GenAtomic\Optimize\Macro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cd0e7a053322a97/Documents/GenAtomic/Optimize/Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AECB17-B799-44EB-B6FF-C266041B7D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{63AECB17-B799-44EB-B6FF-C266041B7D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{555C5550-819D-45D9-8AB4-5BA97A263715}"/>
   <bookViews>
-    <workbookView xWindow="2644" yWindow="600" windowWidth="12343" windowHeight="6677" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="1" r:id="rId1"/>
@@ -673,7 +673,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
@@ -724,7 +724,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.85">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -751,14 +751,14 @@
         <v>11</v>
       </c>
       <c r="I2" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="K2" s="2">
         <f>_1st_ref</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
@@ -792,7 +792,7 @@
       </c>
       <c r="K3" s="2">
         <f>K2+Param_Count</f>
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L3" s="2">
         <v>2</v>
@@ -826,13 +826,13 @@
       </c>
       <c r="K4" s="2">
         <f>K3+Param_Count</f>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="L4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="5" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -860,13 +860,13 @@
       </c>
       <c r="K5" s="2">
         <f>K4+Param_Count</f>
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L5" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="6" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -894,13 +894,13 @@
       </c>
       <c r="K6" s="2">
         <f>K5+Param_Count</f>
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L6" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="7" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -927,13 +927,13 @@
       </c>
       <c r="K7" s="2">
         <f>K6+Param_Count</f>
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L7" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="8" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -950,7 +950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="9" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -962,7 +962,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="10" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -973,7 +973,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="11" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -984,7 +984,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="12" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -995,7 +995,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="13" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="14" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.85">
+    <row r="15" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Moved rows around in Lib files.  Changed back, but not a text file.
</commit_message>
<xml_diff>
--- a/Macro/Reference.xlsx
+++ b/Macro/Reference.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cd0e7a053322a97/Documents/GenAtomic/Optimize/Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{63AECB17-B799-44EB-B6FF-C266041B7D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{555C5550-819D-45D9-8AB4-5BA97A263715}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{63AECB17-B799-44EB-B6FF-C266041B7D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE91C95C-B8AD-4417-A7FF-2D2567357683}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
   </bookViews>
@@ -350,6 +350,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -751,14 +755,14 @@
         <v>11</v>
       </c>
       <c r="I2" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="K2" s="2">
         <f>_1st_ref</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
@@ -792,7 +796,7 @@
       </c>
       <c r="K3" s="2">
         <f>K2+Param_Count</f>
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L3" s="2">
         <v>2</v>
@@ -826,7 +830,7 @@
       </c>
       <c r="K4" s="2">
         <f>K3+Param_Count</f>
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="L4" s="2">
         <v>3</v>
@@ -860,7 +864,7 @@
       </c>
       <c r="K5" s="2">
         <f>K4+Param_Count</f>
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="L5" s="2">
         <v>4</v>
@@ -894,7 +898,7 @@
       </c>
       <c r="K6" s="2">
         <f>K5+Param_Count</f>
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L6" s="2">
         <v>5</v>
@@ -927,7 +931,7 @@
       </c>
       <c r="K7" s="2">
         <f>K6+Param_Count</f>
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L7" s="2">
         <v>6</v>

</xml_diff>

<commit_message>
Graph part works, although the CO2 Tons seems off
</commit_message>
<xml_diff>
--- a/Macro/Reference.xlsx
+++ b/Macro/Reference.xlsx
@@ -1,30 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cd0e7a053322a97/Documents/GenAtomic/Optimize/Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{63AECB17-B799-44EB-B6FF-C266041B7D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE91C95C-B8AD-4417-A7FF-2D2567357683}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{63AECB17-B799-44EB-B6FF-C266041B7D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FAF3948-572B-478F-B5A6-73CBFD9371D7}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Reference" sheetId="1" r:id="rId1"/>
+    <sheet name="Reference" sheetId="4" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_1st_ref">Reference!$I$2</definedName>
+    <definedName name="Billion">Reference!$N$4</definedName>
+    <definedName name="Million">Reference!$N$3</definedName>
+    <definedName name="Mult">[1]Calc!$C$4</definedName>
     <definedName name="NRG_Selections">Reference!$J$2:$J$8</definedName>
     <definedName name="NRG_Table">Reference!$J$2:$L$8</definedName>
     <definedName name="Param_Count">Reference!$H$2</definedName>
+    <definedName name="Param_offset">[1]Calc!$C$5</definedName>
     <definedName name="Param_Table">Reference!$D$2:$G$8</definedName>
-    <definedName name="Params">Reference!$D$2:$D$8</definedName>
-    <definedName name="Region_abbr">Reference!$D$10</definedName>
+    <definedName name="Parameter">[1]Graph!$A$2</definedName>
+    <definedName name="Params">Reference!$D$2:$D$4</definedName>
+    <definedName name="Region">[1]Graph!$A$1</definedName>
+    <definedName name="Region_abbr">[1]Calc!$C$3</definedName>
+    <definedName name="Region_Cost">[1]Cost_Graph!$A$1</definedName>
     <definedName name="Region_lookup">Reference!$A$2:$B$15</definedName>
     <definedName name="Regions">Reference!$A$2:$A$15</definedName>
+    <definedName name="Thousand">Reference!$N$2</definedName>
     <definedName name="To_Long">Reference!$B$2:$C$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -53,7 +64,7 @@
     <author>Cliff Gold</author>
   </authors>
   <commentList>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{6B892390-104E-4FF7-9D6B-0FB3DAB4C833}">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{EA4D4957-F324-42A9-B268-A5B75D101284}">
       <text>
         <r>
           <rPr>
@@ -77,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{509D4E4D-4320-4925-9A09-440A1A2BE74A}">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{1292026F-555F-4FE6-A7AE-C2FCE2E82A82}">
       <text>
         <r>
           <rPr>
@@ -105,8 +116,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>Texas</t>
   </si>
@@ -156,9 +189,6 @@
     <t>MIDW</t>
   </si>
   <si>
-    <t>Storage</t>
-  </si>
-  <si>
     <t>MTons</t>
   </si>
   <si>
@@ -177,9 +207,6 @@
     <t>B$</t>
   </si>
   <si>
-    <t>CO2_Cost</t>
-  </si>
-  <si>
     <t>Florida</t>
   </si>
   <si>
@@ -189,9 +216,6 @@
     <t>Gas</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Central</t>
   </si>
   <si>
@@ -204,9 +228,6 @@
     <t>TWh</t>
   </si>
   <si>
-    <t>Supply</t>
-  </si>
-  <si>
     <t>Carolinas</t>
   </si>
   <si>
@@ -216,9 +237,6 @@
     <t>Wind</t>
   </si>
   <si>
-    <t>Energy</t>
-  </si>
-  <si>
     <t>California</t>
   </si>
   <si>
@@ -231,9 +249,6 @@
     <t>GW</t>
   </si>
   <si>
-    <t>Capacity</t>
-  </si>
-  <si>
     <t>Entire US</t>
   </si>
   <si>
@@ -271,6 +286,36 @@
   </si>
   <si>
     <t>NRG Table</t>
+  </si>
+  <si>
+    <t>Capacity GW</t>
+  </si>
+  <si>
+    <t>Thousand</t>
+  </si>
+  <si>
+    <t>Energy TWh</t>
+  </si>
+  <si>
+    <t>Million</t>
+  </si>
+  <si>
+    <t>Billion</t>
+  </si>
+  <si>
+    <t>Capital Cost</t>
+  </si>
+  <si>
+    <t>Fixed Cost</t>
+  </si>
+  <si>
+    <t>Variable Cost</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>CO2 Cost</t>
   </si>
 </sst>
 </file>
@@ -327,12 +372,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -350,6 +401,67 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Graph"/>
+      <sheetName val="Cost_Graph"/>
+      <sheetName val="Calc"/>
+      <sheetName val="Cost_Calc"/>
+      <sheetName val="Reference"/>
+      <sheetName val="Inbox"/>
+      <sheetName val="CAL"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>California</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Capacity GW</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>California</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>CAL</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="C4">
+            <v>1E-3</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="C5">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -672,12 +784,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200BB87E-1EE1-4FF4-A940-43E30C2581DF}">
-  <sheetPr codeName="Sheet16"/>
-  <dimension ref="A1:L15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB90355-6987-4C33-9EAD-98515261771F}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
@@ -688,256 +800,277 @@
     <col min="6" max="6" width="8.265625" style="2" customWidth="1"/>
     <col min="7" max="7" width="9.15234375" style="2" customWidth="1"/>
     <col min="8" max="8" width="10.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.921875" style="2"/>
+    <col min="9" max="13" width="8.921875" style="2"/>
+    <col min="14" max="14" width="12.15234375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.921875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.85">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="str">
         <f>A1</f>
         <v>Regions</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.85">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.85">
-      <c r="A2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="E2" s="2">
         <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="2">
-        <f>1/1000</f>
+        <v>35</v>
+      </c>
+      <c r="G2" s="2" cm="1">
+        <f t="array" ref="G2">1/Thousand</f>
         <v>1E-3</v>
       </c>
       <c r="H2" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" s="2">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K2" s="2">
         <f>_1st_ref</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="29.15" x14ac:dyDescent="0.85">
+      <c r="M2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2">
+        <f>1/Million</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="G3" s="2">
-        <f>1/1000000</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="K3" s="2">
         <f>K2+Param_Count</f>
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="L3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="43.9" x14ac:dyDescent="0.85">
+      <c r="M3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="4">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="G4" s="2">
-        <f>1/1000000</f>
-        <v>9.9999999999999995E-7</v>
+        <v>1</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K4" s="2">
         <f>K3+Param_Count</f>
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="L4" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="M4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="4">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" s="2">
-        <f>1/1000</f>
+        <f>1/Thousand</f>
         <v>1E-3</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K5" s="2">
         <f>K4+Param_Count</f>
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="L5" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E6" s="2">
         <v>4</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2">
-        <f>1/1000</f>
+        <f>1/Thousand</f>
         <v>1E-3</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K6" s="2">
         <f>K5+Param_Count</f>
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="L6" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="E7" s="2">
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="G7" s="2">
-        <v>1</v>
+        <f>1/Thousand</f>
+        <v>1E-3</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="K7" s="2">
         <f>K6+Param_Count</f>
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="L7" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -947,14 +1080,27 @@
       <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2">
+        <f>1/Thousand</f>
+        <v>1E-3</v>
+      </c>
       <c r="J8" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="L8" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -964,9 +1110,8 @@
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -976,8 +1121,9 @@
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -987,8 +1133,9 @@
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -998,8 +1145,9 @@
       <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -1009,8 +1157,9 @@
       <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1020,8 +1169,9 @@
       <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="14.65" x14ac:dyDescent="0.85">
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.85">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1031,6 +1181,19 @@
       <c r="C15" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.85">
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.85">
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.85">
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.85">
+      <c r="G19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed bugs, esp. in Specs.  Got graphs looking good (except bar graphs).
</commit_message>
<xml_diff>
--- a/Macro/Reference.xlsx
+++ b/Macro/Reference.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7cd0e7a053322a97/Documents/GenAtomic/Optimize/Macro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{63AECB17-B799-44EB-B6FF-C266041B7D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FAF3948-572B-478F-B5A6-73CBFD9371D7}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{63AECB17-B799-44EB-B6FF-C266041B7D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{933CE4FA-9CB1-41E2-8516-077E31E2CD69}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="16637" windowHeight="9437" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C81145A1-E574-4696-BBD3-79E862FF097E}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference" sheetId="4" r:id="rId1"/>
@@ -27,9 +27,9 @@
     <definedName name="NRG_Table">Reference!$J$2:$L$8</definedName>
     <definedName name="Param_Count">Reference!$H$2</definedName>
     <definedName name="Param_offset">[1]Calc!$C$5</definedName>
-    <definedName name="Param_Table">Reference!$D$2:$G$8</definedName>
+    <definedName name="Param_Table">Reference!$D$2:$G$9</definedName>
     <definedName name="Parameter">[1]Graph!$A$2</definedName>
-    <definedName name="Params">Reference!$D$2:$D$4</definedName>
+    <definedName name="Params">Reference!$D$2:$D$5</definedName>
     <definedName name="Region">[1]Graph!$A$1</definedName>
     <definedName name="Region_abbr">[1]Calc!$C$3</definedName>
     <definedName name="Region_Cost">[1]Cost_Graph!$A$1</definedName>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>Texas</t>
   </si>
@@ -316,6 +316,12 @@
   </si>
   <si>
     <t>CO2 Cost</t>
+  </si>
+  <si>
+    <t>Max_Build</t>
+  </si>
+  <si>
+    <t>PCT</t>
   </si>
 </sst>
 </file>
@@ -786,26 +792,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AB90355-6987-4C33-9EAD-98515261771F}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.85"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="12.07421875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="14.69140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="1.65234375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.265625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.15234375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="8.921875" style="2"/>
-    <col min="14" max="14" width="12.15234375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.921875" style="2"/>
+    <col min="1" max="3" width="12.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="2" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="13" width="8.85546875" style="2"/>
+    <col min="14" max="14" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="29.15" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -843,7 +849,7 @@
       </c>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>36</v>
       </c>
@@ -889,7 +895,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -929,7 +935,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -943,7 +949,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>16</v>
@@ -968,7 +974,7 @@
         <v>1000000000</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -979,17 +985,16 @@
         <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="E5" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="G5" s="2">
-        <f>1/Thousand</f>
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>24</v>
@@ -1002,7 +1007,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -1013,10 +1018,10 @@
         <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>21</v>
@@ -1036,7 +1041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -1047,10 +1052,10 @@
         <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>21</v>
@@ -1070,7 +1075,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1081,10 +1086,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E8" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>21</v>
@@ -1100,7 +1105,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1110,8 +1115,21 @@
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.85">
+      <c r="D9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="2">
+        <f>1/Thousand</f>
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1121,9 +1139,8 @@
       <c r="C10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G10"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.85">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1135,7 +1152,7 @@
       </c>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1147,7 +1164,7 @@
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>4</v>
       </c>
@@ -1159,7 +1176,7 @@
       </c>
       <c r="G13"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -1171,7 +1188,7 @@
       </c>
       <c r="G14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
@@ -1183,17 +1200,20 @@
       </c>
       <c r="G15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.85">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G16"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.85">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.85">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G18"/>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.85">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G19"/>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>